<commit_message>
Deleting Role Enumeration from SBEO
</commit_message>
<xml_diff>
--- a/Things to do.xlsx
+++ b/Things to do.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qasim KHALID\Dropbox\Qasim's Progress\My Ontologies\SBEO_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFED4A3-0C86-4A93-9FE9-10DFA3D66B4C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACE6697-C82B-461A-998D-47D80472B7FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19590" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="25 Sept 2020" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Ontology</t>
   </si>
@@ -72,10 +72,16 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Figures update</t>
-  </si>
-  <si>
-    <t>Tables update</t>
+    <t>Updating w.r.t. role in context pattern (30 mins)</t>
+  </si>
+  <si>
+    <t>Updating w.r.t. sensors (30 mins)</t>
+  </si>
+  <si>
+    <t>Figures update (30 mins)</t>
+  </si>
+  <si>
+    <t>Tables update (30 mins)</t>
   </si>
 </sst>
 </file>
@@ -107,15 +113,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -136,15 +154,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -155,15 +164,52 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -171,7 +217,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -181,68 +227,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -251,7 +238,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -259,100 +257,61 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -629,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -641,181 +600,178 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="7"/>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="D9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="D10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="7"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Updated Figure and SBEO.owl
</commit_message>
<xml_diff>
--- a/Things to do.xlsx
+++ b/Things to do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qasim KHALID\Dropbox\Qasim's Progress\My Ontologies\SBEO_Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACE6697-C82B-461A-998D-47D80472B7FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB36EC54-B46B-4F12-81DF-C63D48305813}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19590" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -275,31 +275,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +590,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,26 +601,26 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -628,13 +629,13 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -648,10 +649,10 @@
       <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="11" t="s">
         <v>5</v>
       </c>
     </row>
@@ -665,7 +666,7 @@
       <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="3"/>
@@ -676,7 +677,7 @@
       <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="18" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="3"/>

</xml_diff>